<commit_message>
changes2 git commit -m changes
</commit_message>
<xml_diff>
--- a/data/Datos_STOXX50_.xlsx
+++ b/data/Datos_STOXX50_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\OneDrive\Escritorio\Personal\CAIXA\Web\Definitivo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iebs-my.sharepoint.com/personal/valentina_bailon_ie_edu/Documents/Escritorio/PROYECTO MÁSTER/ANÁLISIS EUROSTOXX 50/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9895D4-3C59-4EED-88CE-2C5E43A45AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0F9895D4-3C59-4EED-88CE-2C5E43A45AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1B0DA17-9863-4A2A-A08A-62B523665E15}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-610" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Financiero" sheetId="1" r:id="rId1"/>
@@ -872,766 +872,766 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ABW23"/>
   <sheetViews>
-    <sheetView topLeftCell="LP1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="LT1" sqref="LT1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="24" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="21" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="24" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="19" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="24" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="24" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="21" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="24" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="19" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="24" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="24" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="21" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="24" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="19" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="24" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="24" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="21" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="24" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="19" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="24" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="24" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="21" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="24" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="19" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="24" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="24" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="21" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="24" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="109" max="109" width="19" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="24" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="115" max="115" width="24" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="21" bestFit="1" customWidth="1"/>
     <col min="120" max="120" width="24" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="124" max="124" width="19" bestFit="1" customWidth="1"/>
     <col min="125" max="125" width="24" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="130" max="130" width="24" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="134" max="134" width="21" bestFit="1" customWidth="1"/>
     <col min="135" max="135" width="24" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="139" max="139" width="19" bestFit="1" customWidth="1"/>
     <col min="140" max="140" width="24" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="145" max="145" width="24" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="149" max="149" width="21" bestFit="1" customWidth="1"/>
     <col min="150" max="150" width="24" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="154" max="154" width="19" bestFit="1" customWidth="1"/>
     <col min="155" max="155" width="24" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="160" max="160" width="24" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="164" max="164" width="21" bestFit="1" customWidth="1"/>
     <col min="165" max="165" width="24" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="169" max="169" width="19" bestFit="1" customWidth="1"/>
     <col min="170" max="170" width="24" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="175" max="175" width="24" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="179" max="179" width="21" bestFit="1" customWidth="1"/>
     <col min="180" max="180" width="24" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="184" max="184" width="19" bestFit="1" customWidth="1"/>
     <col min="185" max="185" width="24" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="190" max="190" width="24" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="194" max="194" width="21" bestFit="1" customWidth="1"/>
     <col min="195" max="195" width="24" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="199" max="199" width="19" bestFit="1" customWidth="1"/>
     <col min="200" max="200" width="24" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="205" max="205" width="24" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="209" max="209" width="21" bestFit="1" customWidth="1"/>
     <col min="210" max="210" width="24" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="214" max="214" width="19" bestFit="1" customWidth="1"/>
     <col min="215" max="215" width="24" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="220" max="220" width="24" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="224" max="224" width="21" bestFit="1" customWidth="1"/>
     <col min="225" max="225" width="24" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="229" max="229" width="19" bestFit="1" customWidth="1"/>
     <col min="230" max="230" width="24" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="231" max="231" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="232" max="232" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="235" max="235" width="24" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="239" max="239" width="21" bestFit="1" customWidth="1"/>
     <col min="240" max="240" width="24" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="244" max="244" width="19" bestFit="1" customWidth="1"/>
     <col min="245" max="245" width="24" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="249" max="249" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="250" max="250" width="24" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="254" max="254" width="21" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="256" max="256" width="19" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="266" max="266" width="41" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="269" max="269" width="21" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="271" max="271" width="19" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="280" max="280" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="273" max="273" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="275" max="275" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="279" max="279" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="281" max="281" width="41" bestFit="1" customWidth="1"/>
-    <col min="282" max="282" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="283" max="283" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="282" max="282" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="283" max="283" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="284" max="284" width="21" bestFit="1" customWidth="1"/>
-    <col min="285" max="285" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="285" max="285" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="286" max="286" width="19" bestFit="1" customWidth="1"/>
-    <col min="287" max="287" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="288" max="288" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="289" max="289" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="290" max="290" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="291" max="291" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="292" max="292" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="293" max="293" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="294" max="294" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="295" max="295" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="287" max="287" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="288" max="288" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="289" max="289" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="290" max="290" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="291" max="291" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="292" max="292" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="293" max="293" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="294" max="294" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="295" max="295" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="296" max="296" width="41" bestFit="1" customWidth="1"/>
-    <col min="297" max="297" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="298" max="298" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="297" max="297" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="299" max="299" width="21" bestFit="1" customWidth="1"/>
-    <col min="300" max="300" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="300" max="300" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="301" max="301" width="19" bestFit="1" customWidth="1"/>
-    <col min="302" max="302" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="303" max="303" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="304" max="304" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="305" max="305" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="306" max="306" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="307" max="307" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="308" max="308" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="309" max="309" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="310" max="310" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="302" max="302" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="303" max="303" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="304" max="304" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="305" max="305" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="306" max="306" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="307" max="307" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="308" max="308" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="309" max="309" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="310" max="310" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="311" max="311" width="41" bestFit="1" customWidth="1"/>
-    <col min="312" max="312" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="313" max="313" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="312" max="312" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="313" max="313" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="314" max="314" width="21" bestFit="1" customWidth="1"/>
-    <col min="315" max="315" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="315" max="315" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="316" max="316" width="19" bestFit="1" customWidth="1"/>
-    <col min="317" max="317" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="318" max="318" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="319" max="319" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="320" max="320" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="321" max="321" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="322" max="322" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="323" max="323" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="324" max="324" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="325" max="325" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="317" max="317" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="318" max="318" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="319" max="319" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="320" max="320" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="321" max="321" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="322" max="322" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="323" max="323" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="324" max="324" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="325" max="325" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="326" max="326" width="41" bestFit="1" customWidth="1"/>
-    <col min="327" max="327" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="328" max="328" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="327" max="327" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="328" max="328" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="329" max="329" width="21" bestFit="1" customWidth="1"/>
-    <col min="330" max="330" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="330" max="330" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="331" max="331" width="19" bestFit="1" customWidth="1"/>
-    <col min="332" max="332" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="333" max="333" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="334" max="334" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="335" max="335" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="336" max="336" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="337" max="337" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="338" max="338" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="339" max="339" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="340" max="340" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="332" max="332" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="333" max="333" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="334" max="334" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="335" max="335" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="336" max="336" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="337" max="337" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="338" max="338" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="339" max="339" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="340" max="340" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="341" max="341" width="41" bestFit="1" customWidth="1"/>
-    <col min="342" max="342" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="343" max="343" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="342" max="342" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="343" max="343" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="344" max="344" width="21" bestFit="1" customWidth="1"/>
-    <col min="345" max="345" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="345" max="345" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="346" max="346" width="19" bestFit="1" customWidth="1"/>
-    <col min="347" max="347" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="348" max="348" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="349" max="349" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="350" max="350" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="351" max="351" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="352" max="352" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="353" max="353" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="354" max="354" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="355" max="355" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="347" max="347" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="348" max="348" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="349" max="349" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="350" max="350" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="351" max="351" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="352" max="352" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="353" max="353" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="354" max="354" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="355" max="355" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="356" max="356" width="41" bestFit="1" customWidth="1"/>
-    <col min="357" max="357" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="358" max="358" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="357" max="357" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="358" max="358" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="359" max="359" width="21" bestFit="1" customWidth="1"/>
-    <col min="360" max="360" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="360" max="360" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="361" max="361" width="19" bestFit="1" customWidth="1"/>
-    <col min="362" max="362" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="363" max="363" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="364" max="364" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="365" max="365" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="366" max="366" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="367" max="367" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="368" max="368" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="369" max="369" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="370" max="370" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="362" max="362" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="363" max="363" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="364" max="364" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="365" max="365" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="366" max="366" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="367" max="367" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="368" max="368" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="369" max="369" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="370" max="370" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="371" max="371" width="41" bestFit="1" customWidth="1"/>
-    <col min="372" max="372" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="373" max="373" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="372" max="372" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="373" max="373" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="374" max="374" width="21" bestFit="1" customWidth="1"/>
-    <col min="375" max="375" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="375" max="375" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="376" max="376" width="19" bestFit="1" customWidth="1"/>
-    <col min="377" max="377" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="378" max="378" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="379" max="379" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="380" max="380" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="381" max="381" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="382" max="382" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="383" max="383" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="384" max="384" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="385" max="385" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="377" max="377" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="378" max="378" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="379" max="379" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="380" max="380" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="381" max="381" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="382" max="382" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="383" max="383" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="384" max="384" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="385" max="385" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="386" max="386" width="41" bestFit="1" customWidth="1"/>
-    <col min="387" max="387" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="388" max="388" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="387" max="387" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="388" max="388" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="389" max="389" width="21" bestFit="1" customWidth="1"/>
-    <col min="390" max="390" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="390" max="390" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="391" max="391" width="19" bestFit="1" customWidth="1"/>
-    <col min="392" max="392" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="393" max="393" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="394" max="394" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="395" max="395" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="396" max="396" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="397" max="397" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="398" max="398" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="399" max="399" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="400" max="400" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="392" max="392" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="393" max="393" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="394" max="394" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="395" max="395" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="396" max="396" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="397" max="397" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="398" max="398" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="399" max="399" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="400" max="400" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="401" max="401" width="41" bestFit="1" customWidth="1"/>
-    <col min="402" max="402" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="403" max="403" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="402" max="402" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="403" max="403" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="404" max="404" width="21" bestFit="1" customWidth="1"/>
-    <col min="405" max="405" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="405" max="405" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="406" max="406" width="19" bestFit="1" customWidth="1"/>
-    <col min="407" max="407" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="408" max="408" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="409" max="409" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="410" max="410" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="411" max="411" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="412" max="412" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="413" max="413" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="414" max="414" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="415" max="415" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="407" max="407" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="408" max="408" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="409" max="409" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="410" max="410" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="411" max="411" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="412" max="412" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="413" max="413" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="414" max="414" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="415" max="415" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="416" max="416" width="41" bestFit="1" customWidth="1"/>
-    <col min="417" max="417" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="418" max="418" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="417" max="417" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="418" max="418" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="419" max="419" width="21" bestFit="1" customWidth="1"/>
-    <col min="420" max="420" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="420" max="420" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="421" max="421" width="19" bestFit="1" customWidth="1"/>
-    <col min="422" max="422" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="423" max="423" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="424" max="424" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="425" max="425" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="426" max="426" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="427" max="427" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="428" max="428" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="429" max="429" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="430" max="430" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="422" max="422" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="423" max="423" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="424" max="424" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="425" max="425" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="426" max="426" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="427" max="427" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="428" max="428" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="429" max="429" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="430" max="430" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="431" max="431" width="41" bestFit="1" customWidth="1"/>
-    <col min="432" max="432" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="433" max="433" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="432" max="432" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="433" max="433" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="434" max="434" width="21" bestFit="1" customWidth="1"/>
-    <col min="435" max="435" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="435" max="435" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="436" max="436" width="19" bestFit="1" customWidth="1"/>
-    <col min="437" max="437" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="438" max="438" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="439" max="439" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="440" max="440" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="441" max="441" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="442" max="442" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="443" max="443" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="444" max="444" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="445" max="445" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="437" max="437" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="438" max="438" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="439" max="439" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="440" max="440" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="441" max="441" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="442" max="442" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="443" max="443" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="444" max="444" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="445" max="445" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="446" max="446" width="41" bestFit="1" customWidth="1"/>
-    <col min="447" max="447" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="448" max="448" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="447" max="447" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="448" max="448" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="449" max="449" width="21" bestFit="1" customWidth="1"/>
-    <col min="450" max="450" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="450" max="450" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="451" max="451" width="19" bestFit="1" customWidth="1"/>
-    <col min="452" max="452" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="453" max="453" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="454" max="454" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="455" max="455" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="456" max="456" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="457" max="457" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="458" max="458" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="459" max="459" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="460" max="460" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="452" max="452" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="453" max="453" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="454" max="454" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="455" max="455" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="456" max="456" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="457" max="457" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="458" max="458" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="459" max="459" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="460" max="460" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="461" max="461" width="41" bestFit="1" customWidth="1"/>
-    <col min="462" max="462" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="463" max="463" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="462" max="462" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="463" max="463" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="464" max="464" width="21" bestFit="1" customWidth="1"/>
-    <col min="465" max="465" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="465" max="465" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="466" max="466" width="19" bestFit="1" customWidth="1"/>
-    <col min="467" max="467" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="468" max="468" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="469" max="469" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="470" max="470" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="471" max="471" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="472" max="472" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="473" max="473" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="474" max="474" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="475" max="475" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="467" max="467" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="468" max="468" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="469" max="469" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="470" max="470" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="471" max="471" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="472" max="472" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="473" max="473" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="474" max="474" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="475" max="475" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="476" max="476" width="41" bestFit="1" customWidth="1"/>
-    <col min="477" max="477" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="478" max="478" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="477" max="477" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="478" max="478" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="479" max="479" width="21" bestFit="1" customWidth="1"/>
-    <col min="480" max="480" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="480" max="480" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="481" max="481" width="19" bestFit="1" customWidth="1"/>
-    <col min="482" max="482" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="483" max="483" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="484" max="484" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="485" max="485" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="486" max="486" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="487" max="487" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="488" max="488" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="489" max="489" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="490" max="490" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="482" max="482" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="483" max="483" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="484" max="484" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="485" max="485" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="486" max="486" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="487" max="487" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="488" max="488" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="489" max="489" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="490" max="490" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="491" max="491" width="41" bestFit="1" customWidth="1"/>
-    <col min="492" max="492" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="493" max="493" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="492" max="492" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="493" max="493" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="494" max="494" width="21" bestFit="1" customWidth="1"/>
-    <col min="495" max="495" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="495" max="495" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="496" max="496" width="19" bestFit="1" customWidth="1"/>
-    <col min="497" max="497" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="498" max="498" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="499" max="499" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="500" max="500" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="501" max="501" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="502" max="502" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="503" max="503" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="504" max="504" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="505" max="505" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="497" max="497" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="498" max="498" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="499" max="499" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="500" max="500" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="501" max="501" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="502" max="502" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="503" max="503" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="504" max="504" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="505" max="505" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="506" max="506" width="41" bestFit="1" customWidth="1"/>
-    <col min="507" max="507" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="508" max="508" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="507" max="507" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="508" max="508" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="509" max="509" width="21" bestFit="1" customWidth="1"/>
-    <col min="510" max="510" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="510" max="510" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="511" max="511" width="19" bestFit="1" customWidth="1"/>
-    <col min="512" max="512" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="515" max="515" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="516" max="516" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="517" max="517" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="518" max="518" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="519" max="519" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="512" max="512" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="516" max="516" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="517" max="517" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="518" max="518" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="519" max="519" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="521" max="521" width="41" bestFit="1" customWidth="1"/>
-    <col min="522" max="522" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="523" max="523" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="522" max="522" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="523" max="523" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="524" max="524" width="21" bestFit="1" customWidth="1"/>
-    <col min="525" max="525" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="525" max="525" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="526" max="526" width="19" bestFit="1" customWidth="1"/>
-    <col min="527" max="527" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="528" max="528" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="529" max="529" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="530" max="530" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="531" max="531" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="532" max="532" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="533" max="533" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="534" max="534" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="535" max="535" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="527" max="527" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="528" max="528" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="529" max="529" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="530" max="530" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="531" max="531" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="532" max="532" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="533" max="533" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="534" max="534" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="535" max="535" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="536" max="536" width="41" bestFit="1" customWidth="1"/>
-    <col min="537" max="537" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="538" max="538" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="537" max="537" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="538" max="538" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="539" max="539" width="21" bestFit="1" customWidth="1"/>
-    <col min="540" max="540" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="540" max="540" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="541" max="541" width="19" bestFit="1" customWidth="1"/>
-    <col min="542" max="542" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="543" max="543" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="544" max="544" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="545" max="545" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="546" max="546" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="547" max="547" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="548" max="548" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="549" max="549" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="550" max="550" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="542" max="542" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="543" max="543" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="544" max="544" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="545" max="545" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="546" max="546" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="547" max="547" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="548" max="548" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="549" max="549" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="550" max="550" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="551" max="551" width="41" bestFit="1" customWidth="1"/>
-    <col min="552" max="552" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="553" max="553" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="552" max="552" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="553" max="553" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="554" max="554" width="21" bestFit="1" customWidth="1"/>
-    <col min="555" max="555" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="555" max="555" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="556" max="556" width="19" bestFit="1" customWidth="1"/>
-    <col min="557" max="557" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="558" max="558" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="559" max="559" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="560" max="560" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="561" max="561" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="562" max="562" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="563" max="563" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="564" max="564" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="565" max="565" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="557" max="557" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="558" max="558" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="559" max="559" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="560" max="560" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="561" max="561" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="562" max="562" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="563" max="563" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="564" max="564" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="565" max="565" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="566" max="566" width="41" bestFit="1" customWidth="1"/>
-    <col min="567" max="567" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="568" max="568" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="567" max="567" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="568" max="568" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="569" max="569" width="21" bestFit="1" customWidth="1"/>
-    <col min="570" max="570" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="570" max="570" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="571" max="571" width="19" bestFit="1" customWidth="1"/>
-    <col min="572" max="572" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="573" max="573" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="574" max="574" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="575" max="575" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="576" max="576" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="577" max="577" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="578" max="578" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="579" max="579" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="580" max="580" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="572" max="572" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="573" max="573" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="574" max="574" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="575" max="575" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="576" max="576" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="577" max="577" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="578" max="578" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="579" max="579" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="580" max="580" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="581" max="581" width="41" bestFit="1" customWidth="1"/>
-    <col min="582" max="582" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="583" max="583" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="582" max="582" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="583" max="583" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="584" max="584" width="21" bestFit="1" customWidth="1"/>
-    <col min="585" max="585" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="585" max="585" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="586" max="586" width="19" bestFit="1" customWidth="1"/>
-    <col min="587" max="587" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="588" max="588" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="589" max="589" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="590" max="590" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="591" max="591" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="592" max="592" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="593" max="593" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="594" max="594" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="595" max="595" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="587" max="587" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="588" max="588" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="589" max="589" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="590" max="590" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="591" max="591" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="592" max="592" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="593" max="593" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="594" max="594" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="595" max="595" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="596" max="596" width="41" bestFit="1" customWidth="1"/>
-    <col min="597" max="597" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="598" max="598" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="597" max="597" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="598" max="598" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="599" max="599" width="21" bestFit="1" customWidth="1"/>
-    <col min="600" max="600" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="600" max="600" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="601" max="601" width="19" bestFit="1" customWidth="1"/>
-    <col min="602" max="602" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="603" max="603" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="604" max="604" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="605" max="605" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="606" max="606" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="607" max="607" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="608" max="608" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="609" max="609" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="610" max="610" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="602" max="602" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="603" max="603" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="604" max="604" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="605" max="605" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="606" max="606" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="607" max="607" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="608" max="608" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="609" max="609" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="610" max="610" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="611" max="611" width="41" bestFit="1" customWidth="1"/>
-    <col min="612" max="612" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="613" max="613" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="612" max="612" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="613" max="613" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="614" max="614" width="21" bestFit="1" customWidth="1"/>
-    <col min="615" max="615" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="615" max="615" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="616" max="616" width="19" bestFit="1" customWidth="1"/>
-    <col min="617" max="617" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="618" max="618" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="619" max="619" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="620" max="620" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="621" max="621" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="622" max="622" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="623" max="623" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="624" max="624" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="625" max="625" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="617" max="617" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="618" max="618" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="619" max="619" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="620" max="620" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="621" max="621" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="622" max="622" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="623" max="623" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="624" max="624" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="625" max="625" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="626" max="626" width="41" bestFit="1" customWidth="1"/>
-    <col min="627" max="627" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="628" max="628" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="627" max="627" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="628" max="628" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="629" max="629" width="21" bestFit="1" customWidth="1"/>
-    <col min="630" max="630" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="630" max="630" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="631" max="631" width="19" bestFit="1" customWidth="1"/>
-    <col min="632" max="632" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="633" max="633" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="634" max="634" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="635" max="635" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="636" max="636" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="637" max="637" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="638" max="638" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="639" max="639" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="640" max="640" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="632" max="632" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="633" max="633" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="634" max="634" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="635" max="635" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="636" max="636" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="637" max="637" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="638" max="638" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="639" max="639" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="640" max="640" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="641" max="641" width="41" bestFit="1" customWidth="1"/>
-    <col min="642" max="642" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="643" max="643" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="642" max="642" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="643" max="643" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="644" max="644" width="21" bestFit="1" customWidth="1"/>
-    <col min="645" max="645" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="645" max="645" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="646" max="646" width="19" bestFit="1" customWidth="1"/>
-    <col min="647" max="647" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="648" max="648" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="649" max="649" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="650" max="650" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="651" max="651" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="652" max="652" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="653" max="653" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="654" max="654" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="655" max="655" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="647" max="647" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="648" max="648" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="649" max="649" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="650" max="650" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="651" max="651" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="652" max="652" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="653" max="653" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="654" max="654" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="655" max="655" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="656" max="656" width="41" bestFit="1" customWidth="1"/>
-    <col min="657" max="657" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="658" max="658" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="657" max="657" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="658" max="658" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="659" max="659" width="21" bestFit="1" customWidth="1"/>
-    <col min="660" max="660" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="660" max="660" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="661" max="661" width="19" bestFit="1" customWidth="1"/>
-    <col min="662" max="662" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="663" max="663" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="664" max="664" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="665" max="665" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="666" max="666" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="667" max="667" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="668" max="668" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="669" max="669" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="670" max="670" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="662" max="662" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="663" max="663" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="664" max="664" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="665" max="665" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="666" max="666" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="667" max="667" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="668" max="668" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="669" max="669" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="670" max="670" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="671" max="671" width="41" bestFit="1" customWidth="1"/>
-    <col min="672" max="672" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="673" max="673" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="672" max="672" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="673" max="673" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="674" max="674" width="21" bestFit="1" customWidth="1"/>
-    <col min="675" max="675" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="675" max="675" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="676" max="676" width="19" bestFit="1" customWidth="1"/>
-    <col min="677" max="677" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="678" max="678" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="679" max="679" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="680" max="680" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="681" max="681" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="682" max="682" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="683" max="683" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="684" max="684" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="685" max="685" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="677" max="677" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="678" max="678" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="679" max="679" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="680" max="680" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="681" max="681" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="682" max="682" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="683" max="683" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="684" max="684" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="685" max="685" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="686" max="686" width="41" bestFit="1" customWidth="1"/>
-    <col min="687" max="687" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="688" max="688" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="687" max="687" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="688" max="688" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="689" max="689" width="21" bestFit="1" customWidth="1"/>
-    <col min="690" max="690" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="690" max="690" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="691" max="691" width="19" bestFit="1" customWidth="1"/>
-    <col min="692" max="692" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="693" max="693" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="694" max="694" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="695" max="695" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="696" max="696" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="697" max="697" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="698" max="698" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="699" max="699" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="700" max="700" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="692" max="692" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="693" max="693" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="694" max="694" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="695" max="695" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="696" max="696" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="697" max="697" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="698" max="698" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="699" max="699" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="700" max="700" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="701" max="701" width="41" bestFit="1" customWidth="1"/>
-    <col min="702" max="702" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="703" max="703" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="702" max="702" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="703" max="703" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="704" max="704" width="21" bestFit="1" customWidth="1"/>
-    <col min="705" max="705" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="705" max="705" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="706" max="706" width="19" bestFit="1" customWidth="1"/>
-    <col min="707" max="707" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="708" max="708" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="709" max="709" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="710" max="710" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="711" max="711" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="712" max="712" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="713" max="713" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="714" max="714" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="715" max="715" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="707" max="707" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="708" max="708" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="709" max="709" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="710" max="710" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="711" max="711" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="712" max="712" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="713" max="713" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="714" max="714" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="715" max="715" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="716" max="716" width="41" bestFit="1" customWidth="1"/>
-    <col min="717" max="717" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="718" max="718" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="717" max="717" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="718" max="718" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="719" max="719" width="21" bestFit="1" customWidth="1"/>
-    <col min="720" max="720" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="720" max="720" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="721" max="721" width="19" bestFit="1" customWidth="1"/>
-    <col min="722" max="722" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="723" max="723" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="724" max="724" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="725" max="725" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="726" max="726" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="727" max="727" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="728" max="728" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="729" max="729" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="730" max="730" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="722" max="722" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="723" max="723" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="724" max="724" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="725" max="725" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="726" max="726" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="727" max="727" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="728" max="728" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="729" max="729" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="730" max="730" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="731" max="731" width="41" bestFit="1" customWidth="1"/>
-    <col min="732" max="732" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="733" max="733" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="732" max="732" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="733" max="733" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="734" max="734" width="21" bestFit="1" customWidth="1"/>
-    <col min="735" max="735" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="735" max="735" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="736" max="736" width="19" bestFit="1" customWidth="1"/>
-    <col min="737" max="737" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="738" max="738" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="739" max="739" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="740" max="740" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="741" max="741" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="742" max="742" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="743" max="743" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="744" max="744" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="745" max="745" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="737" max="737" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="738" max="738" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="739" max="739" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="740" max="740" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="741" max="741" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="742" max="742" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="743" max="743" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="744" max="744" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="745" max="745" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="746" max="746" width="41" bestFit="1" customWidth="1"/>
-    <col min="747" max="747" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="748" max="748" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="747" max="747" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="748" max="748" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="749" max="749" width="21" bestFit="1" customWidth="1"/>
-    <col min="750" max="750" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="750" max="750" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="751" max="751" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v xml:space="preserve">WKL NA  </v>
       </c>
     </row>
-    <row r="2" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>42369</v>
       </c>
@@ -9040,7 +9040,7 @@
         <v>11624.4905</v>
       </c>
     </row>
-    <row r="4" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>42735</v>
       </c>
@@ -11295,7 +11295,7 @@
         <v>12772.5996</v>
       </c>
     </row>
-    <row r="5" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43100</v>
       </c>
@@ -13550,7 +13550,7 @@
         <v>15311.576300000001</v>
       </c>
     </row>
-    <row r="6" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>43465</v>
       </c>
@@ -15805,7 +15805,7 @@
         <v>17072.332200000001</v>
       </c>
     </row>
-    <row r="7" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>43830</v>
       </c>
@@ -18060,7 +18060,7 @@
         <v>20443.908100000001</v>
       </c>
     </row>
-    <row r="8" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44196</v>
       </c>
@@ -20315,7 +20315,7 @@
         <v>21231.382600000001</v>
       </c>
     </row>
-    <row r="9" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44561</v>
       </c>
@@ -22570,7 +22570,7 @@
         <v>29879.691200000001</v>
       </c>
     </row>
-    <row r="10" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44926</v>
       </c>
@@ -24825,7 +24825,7 @@
         <v>27929.280599999998</v>
       </c>
     </row>
-    <row r="11" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>45291</v>
       </c>
@@ -27080,7 +27080,7 @@
         <v>34693.765700000004</v>
       </c>
     </row>
-    <row r="12" spans="1:751" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:751" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>45657</v>
       </c>
@@ -29335,7 +29335,7 @@
         <v>41660.306400000001</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G23" s="8"/>
     </row>
   </sheetData>
@@ -29348,266 +29348,266 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC99AA1-7A40-4EDD-A2F3-4FAEFD28DDAF}">
   <dimension ref="A1:IQ12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="24" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="24" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.46484375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="19" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="24" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="19" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="24" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="19" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="24" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="13" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="19" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="24" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="13" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="19" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="24" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="19" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="24" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="19" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="24" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="13" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="19" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="24" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="13" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="19" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="24" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="13" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="19" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="24" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="13" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="19" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="24" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="13" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="19" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="24" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="13" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="19" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="24" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="13" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="19" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="24" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="13" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="19" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="24" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="13" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="109" max="109" width="19" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="24" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="13" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="114" max="114" width="19" bestFit="1" customWidth="1"/>
     <col min="115" max="115" width="24" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="117" max="117" width="13" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="19" bestFit="1" customWidth="1"/>
     <col min="120" max="120" width="24" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="122" max="122" width="13" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="124" max="124" width="19" bestFit="1" customWidth="1"/>
     <col min="125" max="125" width="24" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="13" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="129" max="129" width="19" bestFit="1" customWidth="1"/>
     <col min="130" max="130" width="24" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="132" max="132" width="13" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="134" max="134" width="19" bestFit="1" customWidth="1"/>
     <col min="135" max="135" width="24" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="137" max="137" width="13" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="139" max="139" width="19" bestFit="1" customWidth="1"/>
     <col min="140" max="140" width="24" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="142" max="142" width="13" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="144" max="144" width="19" bestFit="1" customWidth="1"/>
     <col min="145" max="145" width="24" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="147" max="147" width="13" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="149" max="149" width="19" bestFit="1" customWidth="1"/>
     <col min="150" max="150" width="24" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="152" max="152" width="13" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="154" max="154" width="19" bestFit="1" customWidth="1"/>
     <col min="155" max="155" width="24" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="157" max="157" width="13" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="159" max="159" width="19" bestFit="1" customWidth="1"/>
     <col min="160" max="160" width="24" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="162" max="162" width="13" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="164" max="164" width="19" bestFit="1" customWidth="1"/>
     <col min="165" max="165" width="24" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="167" max="167" width="13" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="169" max="169" width="19" bestFit="1" customWidth="1"/>
     <col min="170" max="170" width="24" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="174" max="174" width="19" bestFit="1" customWidth="1"/>
     <col min="175" max="175" width="24" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="179" max="179" width="19" bestFit="1" customWidth="1"/>
     <col min="180" max="180" width="24" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="182" max="182" width="13" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="184" max="184" width="19" bestFit="1" customWidth="1"/>
     <col min="185" max="185" width="24" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="187" max="187" width="13" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="189" max="189" width="19" bestFit="1" customWidth="1"/>
     <col min="190" max="190" width="24" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="192" max="192" width="13" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="194" max="194" width="19" bestFit="1" customWidth="1"/>
     <col min="195" max="195" width="24" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="197" max="197" width="13" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="199" max="199" width="19" bestFit="1" customWidth="1"/>
     <col min="200" max="200" width="24" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="202" max="202" width="13" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="204" max="204" width="19" bestFit="1" customWidth="1"/>
     <col min="205" max="205" width="24" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="207" max="207" width="13" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="209" max="209" width="19" bestFit="1" customWidth="1"/>
     <col min="210" max="210" width="24" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="212" max="212" width="13" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="214" max="214" width="19" bestFit="1" customWidth="1"/>
     <col min="215" max="215" width="24" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="217" max="217" width="13" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="219" max="219" width="19" bestFit="1" customWidth="1"/>
     <col min="220" max="220" width="24" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="224" max="224" width="19" bestFit="1" customWidth="1"/>
     <col min="225" max="225" width="24" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="227" max="227" width="13" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="229" max="229" width="19" bestFit="1" customWidth="1"/>
     <col min="230" max="230" width="24" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="231" max="231" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="232" max="232" width="13" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="234" max="234" width="19" bestFit="1" customWidth="1"/>
     <col min="235" max="235" width="24" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="237" max="237" width="13" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="239" max="239" width="19" bestFit="1" customWidth="1"/>
     <col min="240" max="240" width="24" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="244" max="244" width="19" bestFit="1" customWidth="1"/>
     <col min="245" max="245" width="24" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="247" max="247" width="13" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="249" max="249" width="19" bestFit="1" customWidth="1"/>
     <col min="250" max="250" width="24" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:251" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>94</v>
       </c>
@@ -30559,7 +30559,7 @@
         <v xml:space="preserve">WKL NA  </v>
       </c>
     </row>
-    <row r="2" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -31314,7 +31314,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>42369</v>
       </c>
@@ -32069,7 +32069,7 @@
         <v>2.4300000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>42734</v>
       </c>
@@ -32824,7 +32824,7 @@
         <v>7.31</v>
       </c>
     </row>
-    <row r="5" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43098</v>
       </c>
@@ -33579,7 +33579,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="6" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>43465</v>
       </c>
@@ -34334,7 +34334,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="7" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>43830</v>
       </c>
@@ -35089,7 +35089,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="8" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44196</v>
       </c>
@@ -35844,7 +35844,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="9" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44561</v>
       </c>
@@ -36599,7 +36599,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="10" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44925</v>
       </c>
@@ -37354,7 +37354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>45289</v>
       </c>
@@ -38109,7 +38109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:251" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>45657</v>
       </c>
@@ -38873,19 +38873,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B009C49-6DF1-4ABB-AF34-861A74C28026}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1328125" customWidth="1"/>
-    <col min="3" max="3" width="28.46484375" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>92</v>
       </c>
@@ -38899,7 +38900,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -38917,7 +38918,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -38935,7 +38936,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -38953,7 +38954,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -38971,7 +38972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -38989,7 +38990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -39007,7 +39008,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -39025,7 +39026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -39043,7 +39044,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -39061,7 +39062,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>103</v>
       </c>
@@ -39079,7 +39080,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -39097,7 +39098,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -39115,7 +39116,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -39133,7 +39134,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>107</v>
       </c>
@@ -39151,7 +39152,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -39169,7 +39170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -39187,7 +39188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>110</v>
       </c>
@@ -39205,7 +39206,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>111</v>
       </c>
@@ -39223,7 +39224,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -39241,7 +39242,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>113</v>
       </c>
@@ -39259,7 +39260,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>114</v>
       </c>
@@ -39277,7 +39278,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>115</v>
       </c>
@@ -39295,7 +39296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>116</v>
       </c>
@@ -39313,7 +39314,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -39331,7 +39332,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>118</v>
       </c>
@@ -39349,7 +39350,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -39367,7 +39368,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>120</v>
       </c>
@@ -39385,7 +39386,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -39403,7 +39404,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>122</v>
       </c>
@@ -39421,7 +39422,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>123</v>
       </c>
@@ -39439,7 +39440,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>124</v>
       </c>
@@ -39457,7 +39458,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>125</v>
       </c>
@@ -39475,7 +39476,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>126</v>
       </c>
@@ -39493,7 +39494,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>127</v>
       </c>
@@ -39511,7 +39512,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>128</v>
       </c>
@@ -39529,7 +39530,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -39547,7 +39548,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -39565,7 +39566,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>131</v>
       </c>
@@ -39583,7 +39584,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>132</v>
       </c>
@@ -39601,7 +39602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -39619,7 +39620,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>134</v>
       </c>
@@ -39637,7 +39638,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>135</v>
       </c>
@@ -39655,7 +39656,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>136</v>
       </c>
@@ -39673,7 +39674,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -39691,7 +39692,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>138</v>
       </c>
@@ -39709,7 +39710,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>139</v>
       </c>
@@ -39727,7 +39728,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>140</v>
       </c>
@@ -39745,7 +39746,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>141</v>
       </c>
@@ -39763,7 +39764,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>142</v>
       </c>
@@ -39781,7 +39782,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>143</v>
       </c>

</xml_diff>